<commit_message>
Found a duplicate tutorial for calculating biomass in python. minor difference in names (/hyperspetral-data/calc_biomass_py.md VS. /lidar/calc-biomass_py.md).
the one in /lidar/ by Paul was actually being displayed online, so I moved the other one (by Tristan Goulden) into the tutorials-in-development folder
</commit_message>
<xml_diff>
--- a/processing_code/redesign-FY20-NDS-GitHub-Format.xlsx
+++ b/processing_code/redesign-FY20-NDS-GitHub-Format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olearyd/Git/dev-aten/NEON-Data-Skills/processing_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FC755C-079F-0745-9058-427898023592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C591A09-A2D8-FF4A-B34A-241475929C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site-map" sheetId="1" r:id="rId1"/>
@@ -1087,9 +1087,6 @@
     <t>create_hillshade_from_terrain_raster_py.md</t>
   </si>
   <si>
-    <t>calc_biomass_py.md</t>
-  </si>
-  <si>
     <t>lidar_uncertainty_py.md</t>
   </si>
   <si>
@@ -1172,6 +1169,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>calc-biomass_py.md</t>
   </si>
 </sst>
 </file>
@@ -3410,9 +3410,9 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3441,7 +3441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="16">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="16">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="16">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="16">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="16">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="16">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="16">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="16">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="16">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="16">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="16">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="16">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="16">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="16">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="16">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="16">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="16">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="16">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="16">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="16">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="16">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" ht="16">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="16">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" ht="16">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" ht="16">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" ht="16">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" ht="16">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" ht="16">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" ht="16">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="16">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" ht="16">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" ht="16">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="16">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" ht="16">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" ht="16">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" ht="16">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" ht="16">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" ht="16">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" ht="16">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="16">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" ht="16">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" ht="16">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" ht="16">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>71</v>
       </c>
       <c r="E129" s="12" t="s">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="F129" s="3" t="s">
         <v>259</v>
@@ -5944,7 +5944,7 @@
         <v>62</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F130" s="13" t="s">
         <v>260</v>
@@ -5982,7 +5982,7 @@
         <v>80</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F132" s="13" t="s">
         <v>264</v>
@@ -6050,7 +6050,7 @@
         <v>119</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F136" s="3" t="s">
         <v>265</v>
@@ -6070,7 +6070,7 @@
         <v>119</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F137" s="5" t="s">
         <v>267</v>
@@ -6090,7 +6090,7 @@
         <v>119</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F138" s="5" t="s">
         <v>268</v>
@@ -6110,7 +6110,7 @@
         <v>119</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F139" s="5" t="s">
         <v>269</v>
@@ -6130,7 +6130,7 @@
         <v>119</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F140" s="5" t="s">
         <v>270</v>
@@ -6150,7 +6150,7 @@
         <v>119</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F141" s="5" t="s">
         <v>271</v>
@@ -6170,7 +6170,7 @@
         <v>119</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F142" s="5" t="s">
         <v>273</v>
@@ -6190,7 +6190,7 @@
         <v>119</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F143" s="5" t="s">
         <v>274</v>
@@ -6210,7 +6210,7 @@
         <v>119</v>
       </c>
       <c r="E144" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F144" s="10" t="s">
         <v>275</v>
@@ -6230,7 +6230,7 @@
         <v>122</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F145" s="10" t="s">
         <v>276</v>
@@ -6322,7 +6322,7 @@
         <v>126</v>
       </c>
       <c r="E150" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F150" s="10" t="s">
         <v>282</v>
@@ -6342,7 +6342,7 @@
         <v>126</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>284</v>
@@ -6362,7 +6362,7 @@
         <v>128</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F152" s="13" t="s">
         <v>286</v>
@@ -6382,7 +6382,7 @@
         <v>136</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F153" s="13" t="s">
         <v>288</v>
@@ -6408,32 +6408,32 @@
     </row>
     <row r="157" spans="1:6" ht="13">
       <c r="E157" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="13">
       <c r="E158" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="13">
       <c r="E159" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="161" spans="5:5" ht="13">
       <c r="E161" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="162" spans="5:5" ht="13">
       <c r="E162" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="13">
       <c r="E163" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -6539,7 +6539,7 @@
     <hyperlink ref="E126" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
     <hyperlink ref="E127" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
     <hyperlink ref="E128" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="E129" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="E129" r:id="rId102" display="calc_biomass_py.md" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
     <hyperlink ref="E130" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
     <hyperlink ref="E132" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
     <hyperlink ref="E136" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
@@ -6722,7 +6722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
@@ -6752,7 +6752,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="16">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -7221,9 +7221,9 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7236,22 +7236,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B1" t="s">
         <v>377</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>378</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>379</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>380</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>381</v>
-      </c>
-      <c r="F1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16">
@@ -9170,7 +9170,7 @@
         <v>71</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>259</v>
@@ -9210,7 +9210,7 @@
         <v>62</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F99" s="20" t="s">
         <v>260</v>
@@ -9330,7 +9330,7 @@
         <v>80</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F105" s="20" t="s">
         <v>264</v>
@@ -9350,7 +9350,7 @@
         <v>122</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F106" s="20" t="s">
         <v>276</v>
@@ -9370,7 +9370,7 @@
         <v>128</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F107" s="22" t="s">
         <v>286</v>
@@ -9390,7 +9390,7 @@
         <v>126</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>284</v>
@@ -9410,7 +9410,7 @@
         <v>126</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F109" s="20" t="s">
         <v>282</v>
@@ -9430,7 +9430,7 @@
         <v>136</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F110" s="20" t="s">
         <v>288</v>
@@ -9450,7 +9450,7 @@
         <v>119</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F111" s="20" t="s">
         <v>275</v>
@@ -9470,7 +9470,7 @@
         <v>119</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F112" s="20" t="s">
         <v>267</v>
@@ -9490,7 +9490,7 @@
         <v>119</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F113" s="20" t="s">
         <v>268</v>
@@ -9510,7 +9510,7 @@
         <v>119</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F114" s="20" t="s">
         <v>269</v>
@@ -9530,7 +9530,7 @@
         <v>119</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F115" s="20" t="s">
         <v>270</v>
@@ -9550,7 +9550,7 @@
         <v>119</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F116" s="22" t="s">
         <v>271</v>
@@ -9570,7 +9570,7 @@
         <v>119</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F117" s="20" t="s">
         <v>273</v>
@@ -9590,7 +9590,7 @@
         <v>119</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F118" s="17" t="s">
         <v>274</v>
@@ -9610,7 +9610,7 @@
         <v>119</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>265</v>
@@ -10014,7 +10014,7 @@
     <hyperlink ref="E91" r:id="rId99" xr:uid="{44392B4B-CBDB-4040-B665-51D1374A31A8}"/>
     <hyperlink ref="E92" r:id="rId100" xr:uid="{F11792C1-8B8F-1840-A761-B7C10D422C20}"/>
     <hyperlink ref="E98" r:id="rId101" xr:uid="{8621E92E-9434-374A-B11A-EC23AA3C722C}"/>
-    <hyperlink ref="E97" r:id="rId102" xr:uid="{9E1E0DDA-2715-3F4A-8836-60606ADF9845}"/>
+    <hyperlink ref="E97" r:id="rId102" display="calc_biomass_py.md" xr:uid="{9E1E0DDA-2715-3F4A-8836-60606ADF9845}"/>
     <hyperlink ref="E99" r:id="rId103" xr:uid="{3E1E1688-D24F-9142-9034-B4F7AF9B978F}"/>
     <hyperlink ref="E105" r:id="rId104" xr:uid="{35CF6CF7-4306-EF45-82CF-17374EE9C13C}"/>
     <hyperlink ref="E119" r:id="rId105" xr:uid="{3CE9E2A0-5E00-954E-8B07-3E2F10737D0F}"/>

</xml_diff>